<commit_message>
Added an Alternative Reverse Lookup Approach
</commit_message>
<xml_diff>
--- a/2DLookup.xlsx
+++ b/2DLookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="8_{1889BD54-3CCD-4C3F-BE4D-7881CAA02684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FEE7F98-39AF-4FAE-8EF3-395EB6B236E4}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{1889BD54-3CCD-4C3F-BE4D-7881CAA02684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8B50F43-7DA6-49E2-86B1-D84747911068}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,6 +38,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
   <si>
     <t>FROM:</t>
   </si>
@@ -214,6 +216,9 @@
   </si>
   <si>
     <t>Test Data</t>
+  </si>
+  <si>
+    <t>Alternative Approaches</t>
   </si>
 </sst>
 </file>
@@ -340,7 +345,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +434,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -490,7 +501,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
@@ -498,6 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
@@ -845,6 +856,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Mark Biegert" refreshedDate="45310.33423414352" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="6" xr:uid="{5BA04B22-7455-4FEB-9C74-146E8376D702}">
   <cacheSource type="worksheet">
@@ -924,7 +939,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1216,10 +1231,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:P116"/>
+  <dimension ref="A1:AC116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1267,46 +1282,46 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C7" s="13" t="str" cm="1">
+      <c r="C7" s="12" t="str" cm="1">
         <f t="array" ref="C7:N7">INDEX({"Jan","Feb","Mar","Apr","May","Jun","Jul","Aug","Sep","Oct","Nov","Dec"},{1,2,3,4,5,6,7,8,9,10,11,12})</f>
         <v>Jan</v>
       </c>
-      <c r="D7" s="14" t="str">
+      <c r="D7" s="13" t="str">
         <v>Feb</v>
       </c>
-      <c r="E7" s="14" t="str">
+      <c r="E7" s="13" t="str">
         <v>Mar</v>
       </c>
-      <c r="F7" s="14" t="str">
+      <c r="F7" s="13" t="str">
         <v>Apr</v>
       </c>
-      <c r="G7" s="14" t="str">
+      <c r="G7" s="13" t="str">
         <v>May</v>
       </c>
-      <c r="H7" s="14" t="str">
+      <c r="H7" s="13" t="str">
         <v>Jun</v>
       </c>
-      <c r="I7" s="14" t="str">
+      <c r="I7" s="13" t="str">
         <v>Jul</v>
       </c>
-      <c r="J7" s="14" t="str">
+      <c r="J7" s="13" t="str">
         <v>Aug</v>
       </c>
-      <c r="K7" s="14" t="str">
+      <c r="K7" s="13" t="str">
         <v>Sep</v>
       </c>
-      <c r="L7" s="14" t="str">
+      <c r="L7" s="13" t="str">
         <v>Oct</v>
       </c>
-      <c r="M7" s="14" t="str">
+      <c r="M7" s="13" t="str">
         <v>Nov</v>
       </c>
-      <c r="N7" s="14" t="str">
+      <c r="N7" s="13" t="str">
         <v>Dec</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="7">
@@ -1347,7 +1362,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="7">
@@ -1388,7 +1403,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="7">
@@ -1429,7 +1444,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="7">
@@ -1470,7 +1485,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="7">
@@ -1581,7 +1596,7 @@
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="19"/>
+      <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -1616,269 +1631,272 @@
     </row>
     <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="E33" s="18" t="s">
+    <row r="33" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="E33" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G33" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I33" s="18" t="s">
+      <c r="I33" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="J33" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="18" t="s">
+      <c r="K33" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L33" s="18" t="s">
+      <c r="L33" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="M33" s="18" t="s">
+      <c r="M33" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="N33" s="18" t="s">
+      <c r="N33" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="O33" s="18" t="s">
+      <c r="O33" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="P33" s="18" t="s">
+      <c r="P33" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D34" s="17" t="s">
+    <row r="34" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="D34" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="15" t="str" cm="1">
+      <c r="E34" s="14" t="str" cm="1">
         <f t="array" ref="E34:P38">IF(F31=Data_2D,Data_2D,"")</f>
         <v/>
       </c>
-      <c r="F34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="G34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="H34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="I34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="J34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="K34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="L34" s="15">
+      <c r="F34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="G34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="H34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="I34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="J34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="K34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="L34" s="14">
         <v>19</v>
       </c>
-      <c r="M34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="N34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="O34" s="15" t="str">
-        <v/>
-      </c>
-      <c r="P34" s="15" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D35" s="17" t="s">
+      <c r="M34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="N34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="O34" s="14" t="str">
+        <v/>
+      </c>
+      <c r="P34" s="14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="D35" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="F35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="G35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="H35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="I35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="J35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="K35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="L35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="M35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="N35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="O35" s="15" t="str">
-        <v/>
-      </c>
-      <c r="P35" s="15" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D36" s="17" t="s">
+      <c r="E35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="F35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="G35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="H35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="I35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="J35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="K35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="L35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="M35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="N35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="O35" s="14" t="str">
+        <v/>
+      </c>
+      <c r="P35" s="14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="D36" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="F36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="G36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="H36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="I36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="J36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="K36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="L36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="M36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="N36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="O36" s="15" t="str">
-        <v/>
-      </c>
-      <c r="P36" s="15" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D37" s="17" t="s">
+      <c r="E36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="F36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="G36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="H36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="I36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="J36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="K36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="L36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="M36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="N36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="O36" s="14" t="str">
+        <v/>
+      </c>
+      <c r="P36" s="14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="D37" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="F37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="G37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="H37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="I37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="J37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="K37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="L37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="M37" s="15">
+      <c r="E37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="F37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="G37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="H37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="I37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="J37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="K37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="L37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="M37" s="14">
         <v>19</v>
       </c>
-      <c r="N37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="O37" s="15" t="str">
-        <v/>
-      </c>
-      <c r="P37" s="15" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D38" s="17" t="s">
+      <c r="N37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="O37" s="14" t="str">
+        <v/>
+      </c>
+      <c r="P37" s="14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="D38" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="F38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="G38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="H38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="I38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="J38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="K38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="L38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="M38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="N38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="O38" s="15" t="str">
-        <v/>
-      </c>
-      <c r="P38" s="15" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B41" s="16" t="s">
+      <c r="E38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="F38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="G38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="H38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="I38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="J38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="K38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="L38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="M38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="N38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="O38" s="14" t="str">
+        <v/>
+      </c>
+      <c r="P38" s="14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B41" s="15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R41" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E43" t="str" cm="1">
         <f t="array" ref="E43:P47">IF(Data_2D,Month_2D,"")</f>
         <v>Jan</v>
@@ -1916,8 +1934,45 @@
       <c r="P43" t="str">
         <v>Dec</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R43" s="7" t="str" cm="1">
+        <f t="array" ref="R43:AC47">IFERROR(INDEX(D34:D38,IF(F31=_xlfn.ANCHORARRAY(E34),ROW(_xlfn.ANCHORARRAY(E34))-ROW($E$33),"")),"")</f>
+        <v/>
+      </c>
+      <c r="S43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y43" s="7" t="str">
+        <v>A</v>
+      </c>
+      <c r="Z43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AA43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AB43" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AC43" s="7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E44" t="str">
         <v>Jan</v>
       </c>
@@ -1954,8 +2009,44 @@
       <c r="P44" t="str">
         <v>Dec</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AA44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AB44" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AC44" s="7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E45" t="str">
         <v>Jan</v>
       </c>
@@ -1992,8 +2083,44 @@
       <c r="P45" t="str">
         <v>Dec</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AA45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AB45" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AC45" s="7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E46" t="str">
         <v>Jan</v>
       </c>
@@ -2030,8 +2157,44 @@
       <c r="P46" t="str">
         <v>Dec</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z46" s="7" t="str">
+        <v>D</v>
+      </c>
+      <c r="AA46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AB46" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AC46" s="7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E47" t="str">
         <v>Jan</v>
       </c>
@@ -2068,8 +2231,83 @@
       <c r="P47" t="str">
         <v>Dec</v>
       </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="T47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="U47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="V47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="W47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="X47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Y47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="Z47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AA47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AB47" s="7" t="str">
+        <v/>
+      </c>
+      <c r="AC47" s="7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="R48" s="19" t="str" cm="1">
+        <f t="array" ref="R48:AC52">IF(F31=_xlfn.ANCHORARRAY($E$34),$E$33:$P$33,"")</f>
+        <v/>
+      </c>
+      <c r="S48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="T48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="U48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="V48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="W48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="X48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Y48" s="19" t="str">
+        <v>Aug</v>
+      </c>
+      <c r="Z48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AA48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AB48" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AC48" s="19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E49" t="str" cm="1">
         <f t="array" ref="E49:P53">IF(Data_2D,Team_2D,"")</f>
         <v>A</v>
@@ -2107,8 +2345,44 @@
       <c r="P49" t="str">
         <v>A</v>
       </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="S49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="T49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="U49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="V49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="W49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="X49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Y49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Z49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AA49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AB49" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AC49" s="19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E50" t="str">
         <v>B</v>
       </c>
@@ -2145,8 +2419,44 @@
       <c r="P50" t="str">
         <v>B</v>
       </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="S50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="T50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="U50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="V50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="W50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="X50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Y50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Z50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AA50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AB50" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AC50" s="19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E51" t="str">
         <v>C</v>
       </c>
@@ -2183,8 +2493,44 @@
       <c r="P51" t="str">
         <v>C</v>
       </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="S51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="T51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="U51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="V51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="W51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="X51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Y51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Z51" s="19" t="str">
+        <v>Sep</v>
+      </c>
+      <c r="AA51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AB51" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AC51" s="19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E52" t="str">
         <v>D</v>
       </c>
@@ -2221,8 +2567,44 @@
       <c r="P52" t="str">
         <v>D</v>
       </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="R52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="S52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="T52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="U52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="V52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="W52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="X52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Y52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="Z52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AA52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AB52" s="19" t="str">
+        <v/>
+      </c>
+      <c r="AC52" s="19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:29" x14ac:dyDescent="0.2">
       <c r="E53" t="str">
         <v>E</v>
       </c>
@@ -2260,7 +2642,35 @@
         <v>E</v>
       </c>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="Q54" t="s">
+        <v>42</v>
+      </c>
+      <c r="R54" t="str" cm="1">
+        <f t="array" ref="R54:S54">_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN(",",TRUE,_xlfn.ANCHORARRAY(R43)),",")</f>
+        <v>A</v>
+      </c>
+      <c r="S54" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="55" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="G55" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(G56)</f>
+        <v>=FILTER(B57:D116,D57:D116=F31)</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>43</v>
+      </c>
+      <c r="R55" t="str" cm="1">
+        <f t="array" ref="R55:S55">_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN(",",TRUE,_xlfn.ANCHORARRAY(R48)),",")</f>
+        <v>Aug</v>
+      </c>
+      <c r="S55" t="str">
+        <v>Sep</v>
+      </c>
+    </row>
+    <row r="56" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>43</v>
       </c>
@@ -2281,7 +2691,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B57" t="str" cm="1">
         <f t="array" ref="B57:B116">_xlfn.TOCOL(_xlfn.ANCHORARRAY(E43))</f>
         <v>Jan</v>
@@ -2304,7 +2714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B58" t="str">
         <v>Feb</v>
       </c>
@@ -2315,7 +2725,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B59" t="str">
         <v>Mar</v>
       </c>
@@ -2326,7 +2736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B60" t="str">
         <v>Apr</v>
       </c>
@@ -2337,7 +2747,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B61" t="str">
         <v>May</v>
       </c>
@@ -2348,7 +2758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B62" t="str">
         <v>Jun</v>
       </c>
@@ -2359,7 +2769,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B63" t="str">
         <v>Jul</v>
       </c>
@@ -2370,7 +2780,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B64" t="str">
         <v>Aug</v>
       </c>
@@ -2954,7 +3364,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{97955BCF-1190-41E2-B5C1-EEF118AD713C}">
       <formula1>Team_2D</formula1>
     </dataValidation>
@@ -3145,19 +3555,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -3165,11 +3571,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -3177,19 +3582,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -3197,11 +3598,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -3209,19 +3609,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -3229,11 +3625,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -3241,13 +3636,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>